<commit_message>
hypertension analysis - charts added
</commit_message>
<xml_diff>
--- a/exports/med-prescribed-chart.xlsx
+++ b/exports/med-prescribed-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nari\hyper-sql-analysis\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F01CDB1D-63D8-465C-AF7D-644FC1DCC741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84AB4A5-47D3-48B2-B6D9-DF084C751727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD125EEF-7838-4543-A07F-2D9C3EAD253E}"/>
   </bookViews>
@@ -2073,15 +2073,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2450,9 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7BBEB1-6569-483A-9AB2-4E29DEB64EB4}">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B128"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>